<commit_message>
libellé tra clé rsa
</commit_message>
<xml_diff>
--- a/formats/excel/Formats TRA MCO xx.xlsx
+++ b/formats/excel/Formats TRA MCO xx.xlsx
@@ -1,124 +1,455 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/R/pmeasyr_/R/formats/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="460" windowWidth="27340" windowHeight="17540" tabRatio="500"/>
+    <workbookView windowWidth="24240" windowHeight="12855" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>longueur</t>
+  </si>
+  <si>
+    <t>verif</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>libelle</t>
+  </si>
   <si>
     <t>CLE_RSA</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Clé RSA</t>
+  </si>
+  <si>
     <t>NORSS</t>
   </si>
   <si>
+    <t xml:space="preserve">Numéro de RSS </t>
+  </si>
+  <si>
+    <t>NO_ligne_RSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numéro de ligne dans fichier RSS épuré </t>
+  </si>
+  <si>
     <t>NAS</t>
   </si>
   <si>
+    <t xml:space="preserve">N° administratif de séjour </t>
+  </si>
+  <si>
     <t>DTENT</t>
   </si>
   <si>
+    <t xml:space="preserve">Date d’entrée </t>
+  </si>
+  <si>
+    <t>GHM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHM (d’origine) </t>
+  </si>
+  <si>
     <t>DTSORT</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>nom</t>
-  </si>
-  <si>
-    <t>longueur</t>
-  </si>
-  <si>
-    <t>verif</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>libelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° Index RSA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numéro de RSS </t>
-  </si>
-  <si>
-    <t>NO_ligne_RSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numéro de ligne dans fichier RSS épuré </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° administratif de séjour </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date d’entrée </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GHM (d’origine) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Date de sortie </t>
-  </si>
-  <si>
-    <t>GHM1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -126,24 +457,308 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -152,7 +767,7 @@
   <a:themeElements>
     <a:clrScheme name="Bureau">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -190,7 +805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Bureau">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -225,7 +840,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -400,54 +1015,50 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="30.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -457,18 +1068,18 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -478,18 +1089,18 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -499,18 +1110,18 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -520,18 +1131,18 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -541,18 +1152,18 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -562,18 +1173,18 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -583,13 +1194,14 @@
         <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>